<commit_message>
Make figures again to publication
- Run CircaDB analysis
- Run CircadiPy simulations analysis
</commit_message>
<xml_diff>
--- a/src/analysis_examples/circadb/results_jtk/cosinor_10375402_adam19_.xlsx
+++ b/src/analysis_examples/circadb/results_jtk/cosinor_10375402_adam19_.xlsx
@@ -589,7 +589,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[0.3814249956476165, 0.458652450066756]</t>
+          <t>[0.3809578879251784, 0.4591195577891941]</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -603,7 +603,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>[-1.2956318050840796, -1.1195265111891555]</t>
+          <t>[-1.3082107546480026, -1.1069475616252324]</t>
         </is>
       </c>
       <c r="Q2" t="n">
@@ -617,7 +617,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[0.39561400876998903, 0.43931511083231595]</t>
+          <t>[0.3956119468871589, 0.4393171727151461]</t>
         </is>
       </c>
       <c r="U2" t="n">
@@ -630,10 +630,10 @@
         <v>4.589549549549666</v>
       </c>
       <c r="X2" t="n">
-        <v>4.254894894895001</v>
+        <v>4.207087087087193</v>
       </c>
       <c r="Y2" t="n">
-        <v>4.924204204204331</v>
+        <v>4.972012012012139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>